<commit_message>
added images, updated data.js, altered app.js accordingly
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="107">
   <si>
     <t>LOCATION</t>
   </si>
@@ -336,6 +336,15 @@
   </si>
   <si>
     <t>State of Texas</t>
+  </si>
+  <si>
+    <t>CARRIED WEAPON</t>
+  </si>
+  <si>
+    <t>unarmed</t>
+  </si>
+  <si>
+    <t>armed</t>
   </si>
 </sst>
 </file>
@@ -685,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,11 +706,12 @@
     <col min="2" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="104.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="104.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -718,13 +728,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -740,14 +753,17 @@
       <c r="E2" s="1">
         <v>42249</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -763,14 +779,17 @@
       <c r="E3" s="1">
         <v>42250</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -786,14 +805,17 @@
       <c r="E4" s="1">
         <v>42251</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -809,14 +831,17 @@
       <c r="E5" s="1">
         <v>42252</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -832,14 +857,17 @@
       <c r="E6" s="1">
         <v>42255</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -855,14 +883,17 @@
       <c r="E7" s="1">
         <v>42256</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -878,14 +909,17 @@
       <c r="E8" s="1">
         <v>42260</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -901,14 +935,17 @@
       <c r="E9" s="1">
         <v>42263</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="F9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -924,14 +961,17 @@
       <c r="E10" s="1">
         <v>42265</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -947,14 +987,17 @@
       <c r="E11" s="1">
         <v>42268</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -970,14 +1013,17 @@
       <c r="E12" s="1">
         <v>42268</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -993,14 +1039,17 @@
       <c r="E13" s="1">
         <v>42268</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1016,14 +1065,17 @@
       <c r="E14" s="1">
         <v>42270</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1039,14 +1091,17 @@
       <c r="E15" s="1">
         <v>42271</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="F15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1062,14 +1117,17 @@
       <c r="E16" s="1">
         <v>42272</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="F16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>94</v>
       </c>
@@ -1085,14 +1143,17 @@
       <c r="E17" s="1">
         <v>42274</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1108,14 +1169,17 @@
       <c r="E18" s="1">
         <v>42277</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="2" t="s">
+      <c r="F18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1131,14 +1195,15 @@
       <c r="E19" s="1">
         <v>42279</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="1"/>
+      <c r="G19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1154,14 +1219,15 @@
       <c r="E20" s="1">
         <v>42280</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="F20" s="1"/>
+      <c r="G20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1177,14 +1243,15 @@
       <c r="E21" s="1">
         <v>42282</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="1"/>
+      <c r="G21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1200,14 +1267,15 @@
       <c r="E22" s="1">
         <v>42285</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="F22" s="1"/>
+      <c r="G22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1223,14 +1291,15 @@
       <c r="E23" s="1">
         <v>42286</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="F23" s="1"/>
+      <c r="G23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1246,14 +1315,15 @@
       <c r="E24" s="1">
         <v>42292</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="F24" s="1"/>
+      <c r="G24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1269,14 +1339,15 @@
       <c r="E25" s="1">
         <v>42300</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="F25" s="1"/>
+      <c r="G25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1292,14 +1363,15 @@
       <c r="E26" s="1">
         <v>42306</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="F26" s="1"/>
+      <c r="G26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1315,14 +1387,15 @@
       <c r="E27" s="1">
         <v>42307</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="F27" s="1"/>
+      <c r="G27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -1338,14 +1411,15 @@
       <c r="E28" s="1">
         <v>42307</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="F28" s="1"/>
+      <c r="G28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1361,14 +1435,15 @@
       <c r="E29" s="1">
         <v>42307</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="1"/>
+      <c r="G29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -1384,14 +1459,15 @@
       <c r="E30" s="1">
         <v>42307</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="1"/>
+      <c r="G30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -1407,14 +1483,15 @@
       <c r="E31" s="1">
         <v>42307</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="1"/>
+      <c r="G31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1430,14 +1507,15 @@
       <c r="E32" s="1">
         <v>42308</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="F32" s="1"/>
+      <c r="G32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -1453,14 +1531,15 @@
       <c r="E33" s="1">
         <v>42308</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="F33" s="1"/>
+      <c r="G33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H33" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -1476,14 +1555,15 @@
       <c r="E34" s="1">
         <v>42312</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="1"/>
+      <c r="G34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -1499,14 +1579,15 @@
       <c r="E35" s="1">
         <v>42317</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="1"/>
+      <c r="G35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -1522,14 +1603,15 @@
       <c r="E36" s="1">
         <v>42317</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="F36" s="1"/>
+      <c r="G36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1545,14 +1627,15 @@
       <c r="E37" s="1">
         <v>42324</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="1"/>
+      <c r="G37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1568,14 +1651,15 @@
       <c r="E38" s="1">
         <v>42324</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="F38" s="1"/>
+      <c r="G38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -1591,14 +1675,15 @@
       <c r="E39" s="1">
         <v>42324</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="1"/>
+      <c r="G39" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1614,14 +1699,15 @@
       <c r="E40" s="1">
         <v>42325</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="F40" s="1"/>
+      <c r="G40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H40" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -1637,14 +1723,15 @@
       <c r="E41" s="1">
         <v>42325</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F41" s="1"/>
+      <c r="G41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>92</v>
       </c>
@@ -1660,14 +1747,15 @@
       <c r="E42" s="1">
         <v>42325</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="F42" s="1"/>
+      <c r="G42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H42" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>76</v>
       </c>
@@ -1683,14 +1771,15 @@
       <c r="E43" s="1">
         <v>42329</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G43" t="s">
+      <c r="F43" s="1"/>
+      <c r="G43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -1706,14 +1795,15 @@
       <c r="E44" s="1">
         <v>42331</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F44" s="1"/>
+      <c r="G44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -1729,14 +1819,15 @@
       <c r="E45" s="1">
         <v>42336</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F45" s="1"/>
+      <c r="G45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -1752,14 +1843,15 @@
       <c r="E46" s="1">
         <v>42338</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F46" s="1"/>
+      <c r="G46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -1775,15 +1867,28 @@
     <sortCondition ref="E2:E48"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G8" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G18" r:id="rId3"/>
-    <hyperlink ref="G34" r:id="rId4"/>
-    <hyperlink ref="G45" r:id="rId5"/>
-    <hyperlink ref="G12" r:id="rId6"/>
-    <hyperlink ref="G13" r:id="rId7"/>
+    <hyperlink ref="H8" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H18" r:id="rId3"/>
+    <hyperlink ref="H34" r:id="rId4"/>
+    <hyperlink ref="H45" r:id="rId5"/>
+    <hyperlink ref="H12" r:id="rId6"/>
+    <hyperlink ref="H13" r:id="rId7"/>
+    <hyperlink ref="H2" r:id="rId8"/>
+    <hyperlink ref="H4" r:id="rId9"/>
+    <hyperlink ref="H5" r:id="rId10"/>
+    <hyperlink ref="H6" r:id="rId11"/>
+    <hyperlink ref="H7" r:id="rId12"/>
+    <hyperlink ref="H9" r:id="rId13"/>
+    <hyperlink ref="H10" r:id="rId14"/>
+    <hyperlink ref="H11" r:id="rId15"/>
+    <hyperlink ref="H14" r:id="rId16"/>
+    <hyperlink ref="H15" r:id="rId17"/>
+    <hyperlink ref="H16" r:id="rId18"/>
+    <hyperlink ref="H17" r:id="rId19"/>
+    <hyperlink ref="H19" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated data files, changed title, added to data.xls
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="109">
   <si>
     <t>LOCATION</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>armed</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>CENSUS CODE</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -410,6 +416,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -694,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,13 +720,15 @@
     <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="104.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="104.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -727,17 +744,23 @@
       <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -753,17 +776,17 @@
       <c r="E2" s="1">
         <v>42249</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -779,17 +802,17 @@
       <c r="E3" s="1">
         <v>42250</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -805,17 +828,17 @@
       <c r="E4" s="1">
         <v>42251</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -831,17 +854,17 @@
       <c r="E5" s="1">
         <v>42252</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -857,17 +880,17 @@
       <c r="E6" s="1">
         <v>42255</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -883,17 +906,17 @@
       <c r="E7" s="1">
         <v>42256</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -909,17 +932,17 @@
       <c r="E8" s="1">
         <v>42260</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -935,17 +958,17 @@
       <c r="E9" s="1">
         <v>42263</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -961,17 +984,17 @@
       <c r="E10" s="1">
         <v>42265</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -987,17 +1010,17 @@
       <c r="E11" s="1">
         <v>42268</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -1013,17 +1036,17 @@
       <c r="E12" s="1">
         <v>42268</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1039,17 +1062,17 @@
       <c r="E13" s="1">
         <v>42268</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1065,17 +1088,17 @@
       <c r="E14" s="1">
         <v>42270</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1091,17 +1114,17 @@
       <c r="E15" s="1">
         <v>42271</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1117,17 +1140,17 @@
       <c r="E16" s="1">
         <v>42272</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>94</v>
       </c>
@@ -1143,17 +1166,17 @@
       <c r="E17" s="1">
         <v>42274</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1169,17 +1192,17 @@
       <c r="E18" s="1">
         <v>42277</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1195,15 +1218,23 @@
       <c r="E19" s="1">
         <v>42279</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="3" t="s">
+      <c r="F19" s="6">
+        <v>381</v>
+      </c>
+      <c r="G19" s="6">
+        <v>29</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1219,15 +1250,23 @@
       <c r="E20" s="1">
         <v>42280</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="F20" s="6">
+        <v>329</v>
+      </c>
+      <c r="G20" s="6">
+        <v>22</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1243,15 +1282,23 @@
       <c r="E21" s="1">
         <v>42282</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="3" t="s">
+      <c r="F21" s="6">
+        <v>439</v>
+      </c>
+      <c r="G21" s="6">
+        <v>51</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H21" t="s">
+      <c r="J21" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1267,15 +1314,23 @@
       <c r="E22" s="1">
         <v>42285</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="F22" s="6">
+        <v>435</v>
+      </c>
+      <c r="G22" s="6">
+        <v>39</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1291,15 +1346,23 @@
       <c r="E23" s="1">
         <v>42286</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="F23" s="6">
+        <v>201</v>
+      </c>
+      <c r="G23" s="6">
+        <v>22</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1315,15 +1378,23 @@
       <c r="E24" s="1">
         <v>42292</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="F24" s="6">
+        <v>201</v>
+      </c>
+      <c r="G24" s="6">
+        <v>22</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1339,15 +1410,23 @@
       <c r="E25" s="1">
         <v>42300</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="F25" s="6">
+        <v>257</v>
+      </c>
+      <c r="G25" s="6">
+        <v>64</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1363,15 +1442,23 @@
       <c r="E26" s="1">
         <v>42306</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="F26" s="6">
+        <v>107</v>
+      </c>
+      <c r="G26" s="6">
+        <v>55</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1387,15 +1474,23 @@
       <c r="E27" s="1">
         <v>42307</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="F27" s="6">
+        <v>355</v>
+      </c>
+      <c r="G27" s="6">
+        <v>20</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -1411,15 +1506,23 @@
       <c r="E28" s="1">
         <v>42307</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="F28" s="6">
+        <v>113</v>
+      </c>
+      <c r="G28" s="6">
+        <v>66</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1435,15 +1538,23 @@
       <c r="E29" s="1">
         <v>42307</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="3" t="s">
+      <c r="F29" s="6">
+        <v>113</v>
+      </c>
+      <c r="G29" s="6">
+        <v>29</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H29" t="s">
+      <c r="J29" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -1459,15 +1570,23 @@
       <c r="E30" s="1">
         <v>42307</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="3" t="s">
+      <c r="F30" s="6">
+        <v>201</v>
+      </c>
+      <c r="G30" s="6">
+        <v>24</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H30" t="s">
+      <c r="J30" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -1483,15 +1602,23 @@
       <c r="E31" s="1">
         <v>42307</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="3" t="s">
+      <c r="F31" s="6">
+        <v>113</v>
+      </c>
+      <c r="G31" s="6">
+        <v>29</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H31" t="s">
+      <c r="J31" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1507,15 +1634,23 @@
       <c r="E32" s="1">
         <v>42308</v>
       </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="F32" s="6">
+        <v>257</v>
+      </c>
+      <c r="G32" s="6">
+        <v>28</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -1531,15 +1666,23 @@
       <c r="E33" s="1">
         <v>42308</v>
       </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="F33" s="6">
+        <v>309</v>
+      </c>
+      <c r="G33" s="6">
+        <v>25</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -1555,15 +1698,15 @@
       <c r="E34" s="1">
         <v>42312</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="3" t="s">
+      <c r="H34" s="7"/>
+      <c r="I34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -1579,15 +1722,15 @@
       <c r="E35" s="1">
         <v>42317</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="3" t="s">
+      <c r="H35" s="7"/>
+      <c r="I35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H35" t="s">
+      <c r="J35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -1603,15 +1746,15 @@
       <c r="E36" s="1">
         <v>42317</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="H36" s="7"/>
+      <c r="I36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1627,15 +1770,15 @@
       <c r="E37" s="1">
         <v>42324</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="3" t="s">
+      <c r="H37" s="7"/>
+      <c r="I37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H37" t="s">
+      <c r="J37" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1651,15 +1794,15 @@
       <c r="E38" s="1">
         <v>42324</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="H38" s="7"/>
+      <c r="I38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J38" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -1675,15 +1818,15 @@
       <c r="E39" s="1">
         <v>42324</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="3" t="s">
+      <c r="H39" s="7"/>
+      <c r="I39" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H39" t="s">
+      <c r="J39" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1699,15 +1842,15 @@
       <c r="E40" s="1">
         <v>42325</v>
       </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="H40" s="7"/>
+      <c r="I40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -1723,15 +1866,15 @@
       <c r="E41" s="1">
         <v>42325</v>
       </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="3" t="s">
+      <c r="H41" s="7"/>
+      <c r="I41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H41" t="s">
+      <c r="J41" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>92</v>
       </c>
@@ -1747,15 +1890,15 @@
       <c r="E42" s="1">
         <v>42325</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="H42" s="7"/>
+      <c r="I42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J42" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>76</v>
       </c>
@@ -1771,15 +1914,15 @@
       <c r="E43" s="1">
         <v>42329</v>
       </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H43" t="s">
+      <c r="H43" s="7"/>
+      <c r="I43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -1795,15 +1938,15 @@
       <c r="E44" s="1">
         <v>42331</v>
       </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="3" t="s">
+      <c r="H44" s="7"/>
+      <c r="I44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H44" t="s">
+      <c r="J44" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -1819,15 +1962,15 @@
       <c r="E45" s="1">
         <v>42336</v>
       </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="3" t="s">
+      <c r="H45" s="7"/>
+      <c r="I45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="J45" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -1843,15 +1986,15 @@
       <c r="E46" s="1">
         <v>42338</v>
       </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="3" t="s">
+      <c r="H46" s="7"/>
+      <c r="I46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H46" t="s">
+      <c r="J46" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -1867,28 +2010,42 @@
     <sortCondition ref="E2:E48"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H18" r:id="rId3"/>
-    <hyperlink ref="H34" r:id="rId4"/>
-    <hyperlink ref="H45" r:id="rId5"/>
-    <hyperlink ref="H12" r:id="rId6"/>
-    <hyperlink ref="H13" r:id="rId7"/>
-    <hyperlink ref="H2" r:id="rId8"/>
-    <hyperlink ref="H4" r:id="rId9"/>
-    <hyperlink ref="H5" r:id="rId10"/>
-    <hyperlink ref="H6" r:id="rId11"/>
-    <hyperlink ref="H7" r:id="rId12"/>
-    <hyperlink ref="H9" r:id="rId13"/>
-    <hyperlink ref="H10" r:id="rId14"/>
-    <hyperlink ref="H11" r:id="rId15"/>
-    <hyperlink ref="H14" r:id="rId16"/>
-    <hyperlink ref="H15" r:id="rId17"/>
-    <hyperlink ref="H16" r:id="rId18"/>
-    <hyperlink ref="H17" r:id="rId19"/>
-    <hyperlink ref="H19" r:id="rId20"/>
+    <hyperlink ref="J8" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J18" r:id="rId3"/>
+    <hyperlink ref="J34" r:id="rId4"/>
+    <hyperlink ref="J45" r:id="rId5"/>
+    <hyperlink ref="J12" r:id="rId6"/>
+    <hyperlink ref="J13" r:id="rId7"/>
+    <hyperlink ref="J2" r:id="rId8"/>
+    <hyperlink ref="J4" r:id="rId9"/>
+    <hyperlink ref="J5" r:id="rId10"/>
+    <hyperlink ref="J6" r:id="rId11"/>
+    <hyperlink ref="J7" r:id="rId12"/>
+    <hyperlink ref="J9" r:id="rId13"/>
+    <hyperlink ref="J10" r:id="rId14"/>
+    <hyperlink ref="J11" r:id="rId15"/>
+    <hyperlink ref="J14" r:id="rId16"/>
+    <hyperlink ref="J15" r:id="rId17"/>
+    <hyperlink ref="J16" r:id="rId18"/>
+    <hyperlink ref="J17" r:id="rId19"/>
+    <hyperlink ref="J19" r:id="rId20"/>
+    <hyperlink ref="J20" r:id="rId21"/>
+    <hyperlink ref="J21" r:id="rId22"/>
+    <hyperlink ref="J22" r:id="rId23"/>
+    <hyperlink ref="J23" r:id="rId24"/>
+    <hyperlink ref="J24" r:id="rId25"/>
+    <hyperlink ref="J25" r:id="rId26"/>
+    <hyperlink ref="J26" r:id="rId27"/>
+    <hyperlink ref="J27" r:id="rId28"/>
+    <hyperlink ref="J28" r:id="rId29"/>
+    <hyperlink ref="J29" r:id="rId30"/>
+    <hyperlink ref="J30" r:id="rId31"/>
+    <hyperlink ref="J32" r:id="rId32"/>
+    <hyperlink ref="J33" r:id="rId33"/>
+    <hyperlink ref="J31" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>